<commit_message>
add soul of id 1000 on stage 1
</commit_message>
<xml_diff>
--- a/stage.xlsx
+++ b/stage.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="18195" windowHeight="11595"/>
+    <workbookView xWindow="480" yWindow="100" windowWidth="18200" windowHeight="11600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -422,7 +427,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="63">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -668,6 +673,10 @@
   </si>
   <si>
     <t>1,addExp,40;1,addCopper,10;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,addExp,10;1,addCopper,10;1,addSoul,1000;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -748,10 +757,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -1039,24 +1048,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="4" width="17.125" customWidth="1"/>
-    <col min="5" max="5" width="29.125" customWidth="1"/>
-    <col min="6" max="6" width="24.875" customWidth="1"/>
-    <col min="7" max="7" width="67.375" customWidth="1"/>
-    <col min="8" max="10" width="19.75" customWidth="1"/>
-    <col min="11" max="11" width="33.875" customWidth="1"/>
-    <col min="12" max="13" width="14.75" customWidth="1"/>
-    <col min="14" max="14" width="23.25" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="7" max="7" width="67.33203125" customWidth="1"/>
+    <col min="8" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="33.83203125" customWidth="1"/>
+    <col min="12" max="13" width="14.6640625" customWidth="1"/>
+    <col min="14" max="14" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -1123,7 +1132,7 @@
         <v>54</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1423,34 +1432,50 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>